<commit_message>
Update plan and assignment
</commit_message>
<xml_diff>
--- a/document/Bảng phân công.xlsx
+++ b/document/Bảng phân công.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Bảng phân công" sheetId="1" r:id="rId1"/>
+    <sheet name="Bảng kế hoạch " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>Nhật</t>
   </si>
@@ -93,9 +94,6 @@
     <t>Xem sách: Nghe audio - Phát, hiển thị ds chương</t>
   </si>
   <si>
-    <t>Hoàn thiện tài liệu phân tích - tổ chức project</t>
-  </si>
-  <si>
     <t>Yêu cầu phi chức năng</t>
   </si>
   <si>
@@ -112,13 +110,94 @@
   </si>
   <si>
     <t>Ràng buộc hệ thống</t>
+  </si>
+  <si>
+    <t>Tuần 4: Hoàn thiện tài liệu phân tích - tổ chức project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuần 5: Thiết kế UI - Frontend </t>
+  </si>
+  <si>
+    <t>Tuần 7-8: Code backend</t>
+  </si>
+  <si>
+    <t>Bảng phân công</t>
+  </si>
+  <si>
+    <t>Bảng kế hoạch</t>
+  </si>
+  <si>
+    <t>Giai đoạn 1</t>
+  </si>
+  <si>
+    <t>Đọc sách</t>
+  </si>
+  <si>
+    <t>Nghe audio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QL sách </t>
+  </si>
+  <si>
+    <t>Đọc online</t>
+  </si>
+  <si>
+    <t>Đọc pfd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download </t>
+  </si>
+  <si>
+    <t>Thêm-xóa-sửa</t>
+  </si>
+  <si>
+    <t>Tìm kiếm- phân trang</t>
+  </si>
+  <si>
+    <t>Danh ngôn</t>
+  </si>
+  <si>
+    <t>Giai đoạn 2</t>
+  </si>
+  <si>
+    <t>QL bình luận</t>
+  </si>
+  <si>
+    <t>QL tác giả</t>
+  </si>
+  <si>
+    <t>QL thể loại</t>
+  </si>
+  <si>
+    <t>QL danh ngôn</t>
+  </si>
+  <si>
+    <t>Giai đoạn 3</t>
+  </si>
+  <si>
+    <t>Hoàn thiện tài liệu báo cáo</t>
+  </si>
+  <si>
+    <t>Bình luận</t>
+  </si>
+  <si>
+    <t>Đánh giá</t>
+  </si>
+  <si>
+    <t>21/3 - 30/4</t>
+  </si>
+  <si>
+    <t>1/5-22/5</t>
+  </si>
+  <si>
+    <t>23/5-29/5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +235,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,8 +273,30 @@
         <fgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -245,34 +361,223 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="5" borderId="12" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="5" borderId="15" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="5" borderId="16" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="5" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="7" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="8">
+    <cellStyle name="40% - Accent6" xfId="7" builtinId="51"/>
+    <cellStyle name="60% - Accent3" xfId="5" builtinId="40"/>
+    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
     <cellStyle name="Accent5" xfId="3" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="6" builtinId="49"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,11 +858,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,373 +872,790 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="J2" t="s">
+      <c r="B3" s="7"/>
+      <c r="J3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K3" s="21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7">
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="14">
         <v>44651</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K4" s="23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
+      <c r="L4" s="24"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="K4" t="s">
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="K5" s="23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
+      <c r="L5" s="24"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="K6" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="14">
         <v>44655</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8">
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
         <v>1</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8">
+      <c r="C14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
         <v>2</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
         <v>3</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
         <v>5</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="8">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
         <v>6</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4"/>
+      <c r="C19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="1">
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="13">
         <v>44662</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="8">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
         <v>1</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <v>2</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
+        <v>4</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <v>5</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <v>6</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="8">
+      <c r="C28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11">
+        <v>44667</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="4">
+        <v>1</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="4">
         <v>2</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="4">
+        <v>4</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
+        <v>5</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
+        <v>6</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="8">
+        <v>44681</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4">
+        <v>1</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="8">
+      <c r="C41" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="4">
+        <v>2</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="4">
         <v>3</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="8">
+      <c r="B43" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
         <v>4</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="8">
+      <c r="B44" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4">
         <v>5</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="8">
+      <c r="B45" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4">
         <v>6</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="B46" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A19:B19"/>
+  <mergeCells count="8">
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update plan for team
</commit_message>
<xml_diff>
--- a/document/Bảng phân công.xlsx
+++ b/document/Bảng phân công.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bảng phân công" sheetId="1" r:id="rId1"/>
-    <sheet name="Bảng kế hoạch " sheetId="2" r:id="rId2"/>
+    <sheet name="Bảng phân công (update 19-5)" sheetId="3" r:id="rId2"/>
+    <sheet name="Bảng kế hoạch " sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="125">
   <si>
     <t>Nhật</t>
   </si>
@@ -187,12 +188,6 @@
     <t>21/3 - 30/4</t>
   </si>
   <si>
-    <t>1/5-22/5</t>
-  </si>
-  <si>
-    <t>23/5-29/5</t>
-  </si>
-  <si>
     <t>Xem danh ngôn, bình luận, đánh giá danh ngôn</t>
   </si>
   <si>
@@ -208,14 +203,207 @@
     <t>Update tài liệu</t>
   </si>
   <si>
-    <t>Xem sách: Đọc online - Hiển thị ds chương, nhận xét- đánh giá, setup project header- footer, chuẩn bị data, hoàn thiện DB</t>
+    <t>Xem sách: Đọc online - Hiển thị ds chương, setup project header- footer, chuẩn bị data, hoàn thiện DB</t>
+  </si>
+  <si>
+    <t>Chú thích:</t>
+  </si>
+  <si>
+    <t>Hoàn thành</t>
+  </si>
+  <si>
+    <t>Chưa xong</t>
+  </si>
+  <si>
+    <t>Đang cập nhật</t>
+  </si>
+  <si>
+    <t>15/5-4/6</t>
+  </si>
+  <si>
+    <t>5/6-11/6</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsibility </t>
+  </si>
+  <si>
+    <t>Anh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March </t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Tuần 9</t>
+  </si>
+  <si>
+    <t>Tuần 10</t>
+  </si>
+  <si>
+    <t>Tuần 11</t>
+  </si>
+  <si>
+    <t>Tuần 12</t>
+  </si>
+  <si>
+    <t>Phân tích project</t>
+  </si>
+  <si>
+    <t>Viết SRS - Đăng nhập + QL sách</t>
+  </si>
+  <si>
+    <t>Viết SRS - Đăng xuất + Xem sách</t>
+  </si>
+  <si>
+    <t>UI - Đăng nhập/ Xuất + Xem sách: chi tiết</t>
+  </si>
+  <si>
+    <t>UI - QL sách</t>
+  </si>
+  <si>
+    <t>UI - Xem sách: nghe audio + đọc online + đọc PDF</t>
+  </si>
+  <si>
+    <t>Phân tích công nghệ</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>UI: Xem sách, đăng nhập, ký</t>
+  </si>
+  <si>
+    <t>QL sách: Hiển thị ds - phân trang</t>
+  </si>
+  <si>
+    <t>Nghe audio, home, list sách</t>
+  </si>
+  <si>
+    <t>List danh ngôn</t>
+  </si>
+  <si>
+    <t>Đọc PDF</t>
+  </si>
+  <si>
+    <t>Đăng nhập, kí, Đọc online, bình luận, đánh giá</t>
+  </si>
+  <si>
+    <t>Code Front end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QL sách: thêm, sửa </t>
+  </si>
+  <si>
+    <t>(update list audio, online)</t>
+  </si>
+  <si>
+    <t>Đọc online - Hiển thị ds chương, hiển thị chương</t>
+  </si>
+  <si>
+    <t>Nghe audio - Phát, hiển thị ds chương</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> QL sách: Hiển thị ds - phân trang, tìm kiếm</t>
+  </si>
+  <si>
+    <t>Đọc PDF + download</t>
+  </si>
+  <si>
+    <t>Code logic back end</t>
+  </si>
+  <si>
+    <t>Danh ngôn: xem, list</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Xem sách: Đọc online - Hiển thị ds chương, hiển thị chương</t>
+  </si>
+  <si>
+    <t>QL thể loại (FE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update git project and complete architecture </t>
+  </si>
+  <si>
+    <t>Fix conflict git</t>
+  </si>
+  <si>
+    <t>Hoàn thiện tài liệu Giai đoạn 1</t>
+  </si>
+  <si>
+    <t>Ràng Buộc hệ thống</t>
+  </si>
+  <si>
+    <t>Architecture design</t>
+  </si>
+  <si>
+    <t>Detail design:QL sách - List, QL sách - chi tiết,  Đăng nhập - xuất</t>
+  </si>
+  <si>
+    <t>Detail design:  Xem sách - đọc online, Xem sách - audio, Xem sách - pdf</t>
+  </si>
+  <si>
+    <t>Chưa cập nhật</t>
+  </si>
+  <si>
+    <t>List loại danh sách + home+bảng sếp hạng</t>
+  </si>
+  <si>
+    <t>Xóa sách + Cập nhật ds online/ebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Upload hình + Cập nhật ds audio</t>
+  </si>
+  <si>
+    <t>Đăng nhập, xuất + Đăng kí</t>
+  </si>
+  <si>
+    <t>Chi tiết sách + Bình luận</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàn thiện tiếp - các chức năng giai đoạn 1, update </t>
+  </si>
+  <si>
+    <t>sequence, activity</t>
+  </si>
+  <si>
+    <t>Thiết kế giai đoạn 2</t>
+  </si>
+  <si>
+    <t>Chưa update document</t>
+  </si>
+  <si>
+    <t>QL tài khoản</t>
+  </si>
+  <si>
+    <t>QL sách yêu thích, markbook  (User)</t>
+  </si>
+  <si>
+    <t>QL Danh ngôn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design UI(adobe and code Frontend), Detail UI, SRS
+</t>
+  </si>
+  <si>
+    <t>Đang tiến hành</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,8 +464,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,8 +553,48 @@
         <fgColor theme="6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -545,8 +812,412 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -557,8 +1228,17 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -601,6 +1281,145 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="8" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="32" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="32" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="36" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="38" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="22" xfId="13" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="22" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="22" xfId="16" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="43" xfId="16" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="47" xfId="16" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="43" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="49" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="21" xfId="12"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="32" xfId="18" applyBorder="1"/>
     <xf numFmtId="16" fontId="4" fillId="5" borderId="12" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -622,22 +1441,96 @@
     <xf numFmtId="16" fontId="4" fillId="5" borderId="16" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="39" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="7" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="39" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="33" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="19" xfId="10" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="11" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="50" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="20" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="9"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="19">
+    <cellStyle name="20% - Accent1" xfId="14" builtinId="30"/>
+    <cellStyle name="20% - Accent5" xfId="17" builtinId="46"/>
+    <cellStyle name="40% - Accent3" xfId="16" builtinId="39"/>
     <cellStyle name="40% - Accent6" xfId="7" builtinId="51"/>
+    <cellStyle name="60% - Accent2" xfId="15" builtinId="36"/>
     <cellStyle name="60% - Accent3" xfId="5" builtinId="40"/>
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
     <cellStyle name="Accent3" xfId="9" builtinId="37"/>
     <cellStyle name="Accent5" xfId="3" builtinId="45"/>
     <cellStyle name="Accent6" xfId="6" builtinId="49"/>
     <cellStyle name="Calculation" xfId="8" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="12" builtinId="23"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="10" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Neutral" xfId="18" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Total" xfId="13" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -917,9 +1810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -929,16 +1822,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
@@ -962,10 +1855,10 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="87"/>
       <c r="J3" s="19" t="s">
         <v>8</v>
       </c>
@@ -1071,6 +1964,9 @@
         <v>17</v>
       </c>
       <c r="H9" s="5"/>
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
@@ -1087,12 +1983,32 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
+      <c r="J10" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J11" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="24"/>
+      <c r="B12" s="87"/>
+      <c r="J12" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
@@ -1199,10 +2115,10 @@
       <c r="H19" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="24"/>
+      <c r="B21" s="87"/>
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
       <c r="E21" s="10"/>
@@ -1228,7 +2144,7 @@
       <c r="B23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="4"/>
@@ -1321,10 +2237,10 @@
     </row>
     <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="26"/>
+      <c r="B30" s="89"/>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
       <c r="E30" s="10"/>
@@ -1333,10 +2249,10 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="27">
+      <c r="A31" s="90">
         <v>44667</v>
       </c>
-      <c r="B31" s="28"/>
+      <c r="B31" s="91"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
@@ -1441,10 +2357,10 @@
       <c r="H37" s="4"/>
     </row>
     <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="24"/>
+      <c r="B39" s="87"/>
       <c r="C39" s="10"/>
       <c r="D39" s="11"/>
       <c r="E39" s="10"/>
@@ -1453,10 +2369,10 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="22">
+      <c r="A40" s="85">
         <v>44681</v>
       </c>
-      <c r="B40" s="22"/>
+      <c r="B40" s="85"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
@@ -1469,9 +2385,9 @@
         <v>1</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="23" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="4"/>
@@ -1480,7 +2396,7 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="J41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1492,14 +2408,14 @@
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="21" t="s">
+      <c r="E42" s="23" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="J42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1512,13 +2428,13 @@
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="23" t="s">
         <v>17</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="J43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1533,11 +2449,11 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="21" t="s">
+      <c r="H44" s="23" t="s">
         <v>17</v>
       </c>
       <c r="J44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1545,13 +2461,13 @@
         <v>5</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="21" t="s">
+      <c r="G45" s="23" t="s">
         <v>17</v>
       </c>
       <c r="H45" s="4"/>
@@ -1590,10 +2506,1707 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BQ75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="BS47" sqref="BS47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" customWidth="1"/>
+    <col min="5" max="5" width="11" style="47" customWidth="1"/>
+    <col min="6" max="8" width="2.77734375" style="40" customWidth="1"/>
+    <col min="9" max="9" width="3.21875" style="35" customWidth="1"/>
+    <col min="10" max="38" width="2.77734375" customWidth="1"/>
+    <col min="39" max="39" width="2.77734375" style="33" customWidth="1"/>
+    <col min="40" max="53" width="2.77734375" customWidth="1"/>
+    <col min="54" max="54" width="2.77734375" style="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="60">
+        <v>28</v>
+      </c>
+      <c r="G1" s="60">
+        <v>29</v>
+      </c>
+      <c r="H1" s="60">
+        <v>30</v>
+      </c>
+      <c r="I1" s="61">
+        <v>31</v>
+      </c>
+      <c r="J1" s="38">
+        <v>1</v>
+      </c>
+      <c r="K1" s="38">
+        <v>2</v>
+      </c>
+      <c r="L1" s="38">
+        <v>3</v>
+      </c>
+      <c r="M1" s="38">
+        <v>4</v>
+      </c>
+      <c r="N1" s="38">
+        <v>5</v>
+      </c>
+      <c r="O1" s="38">
+        <v>6</v>
+      </c>
+      <c r="P1" s="38">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="38">
+        <v>8</v>
+      </c>
+      <c r="R1" s="38">
+        <v>9</v>
+      </c>
+      <c r="S1" s="38">
+        <v>10</v>
+      </c>
+      <c r="T1" s="38">
+        <v>11</v>
+      </c>
+      <c r="U1" s="38">
+        <v>12</v>
+      </c>
+      <c r="V1" s="38">
+        <v>13</v>
+      </c>
+      <c r="W1" s="38">
+        <v>14</v>
+      </c>
+      <c r="X1" s="38">
+        <v>15</v>
+      </c>
+      <c r="Y1" s="38">
+        <v>16</v>
+      </c>
+      <c r="Z1" s="38">
+        <v>17</v>
+      </c>
+      <c r="AA1" s="38">
+        <v>18</v>
+      </c>
+      <c r="AB1" s="38">
+        <v>19</v>
+      </c>
+      <c r="AC1" s="38">
+        <v>20</v>
+      </c>
+      <c r="AD1" s="38">
+        <v>21</v>
+      </c>
+      <c r="AE1" s="38">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="38">
+        <v>23</v>
+      </c>
+      <c r="AG1" s="38">
+        <v>24</v>
+      </c>
+      <c r="AH1" s="38">
+        <v>25</v>
+      </c>
+      <c r="AI1" s="38">
+        <v>26</v>
+      </c>
+      <c r="AJ1" s="38">
+        <v>27</v>
+      </c>
+      <c r="AK1" s="38">
+        <v>28</v>
+      </c>
+      <c r="AL1" s="38">
+        <v>29</v>
+      </c>
+      <c r="AM1" s="38">
+        <v>30</v>
+      </c>
+      <c r="AN1" s="38">
+        <v>1</v>
+      </c>
+      <c r="AO1" s="38">
+        <v>2</v>
+      </c>
+      <c r="AP1" s="38">
+        <v>3</v>
+      </c>
+      <c r="AQ1" s="38">
+        <v>4</v>
+      </c>
+      <c r="AR1" s="38">
+        <v>5</v>
+      </c>
+      <c r="AS1" s="38">
+        <v>6</v>
+      </c>
+      <c r="AT1" s="38">
+        <v>7</v>
+      </c>
+      <c r="AU1" s="38">
+        <v>8</v>
+      </c>
+      <c r="AV1" s="38">
+        <v>9</v>
+      </c>
+      <c r="AW1" s="38">
+        <v>10</v>
+      </c>
+      <c r="AX1" s="38">
+        <v>11</v>
+      </c>
+      <c r="AY1" s="38">
+        <v>12</v>
+      </c>
+      <c r="AZ1" s="38">
+        <v>13</v>
+      </c>
+      <c r="BA1" s="38">
+        <v>14</v>
+      </c>
+      <c r="BB1" s="38">
+        <v>15</v>
+      </c>
+      <c r="BC1" s="38">
+        <v>16</v>
+      </c>
+      <c r="BD1" s="38">
+        <v>17</v>
+      </c>
+      <c r="BE1" s="38">
+        <v>18</v>
+      </c>
+      <c r="BF1" s="38">
+        <v>19</v>
+      </c>
+      <c r="BG1" s="38">
+        <v>20</v>
+      </c>
+      <c r="BH1" s="38">
+        <v>21</v>
+      </c>
+      <c r="BI1" s="38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="45"/>
+      <c r="F2" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="93"/>
+      <c r="W2" s="93"/>
+      <c r="X2" s="93"/>
+      <c r="Y2" s="93"/>
+      <c r="Z2" s="93"/>
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="93"/>
+      <c r="AD2" s="93"/>
+      <c r="AE2" s="93"/>
+      <c r="AF2" s="93"/>
+      <c r="AG2" s="93"/>
+      <c r="AH2" s="93"/>
+      <c r="AI2" s="93"/>
+      <c r="AJ2" s="93"/>
+      <c r="AK2" s="93"/>
+      <c r="AL2" s="93"/>
+      <c r="AM2" s="94"/>
+      <c r="AN2" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO2" s="96"/>
+      <c r="AP2" s="96"/>
+      <c r="AQ2" s="96"/>
+      <c r="AR2" s="96"/>
+      <c r="AS2" s="96"/>
+      <c r="AT2" s="96"/>
+      <c r="AU2" s="96"/>
+      <c r="AV2" s="96"/>
+      <c r="AW2" s="96"/>
+      <c r="AX2" s="96"/>
+      <c r="AY2" s="96"/>
+      <c r="AZ2" s="96"/>
+      <c r="BA2" s="96"/>
+      <c r="BB2" s="97"/>
+    </row>
+    <row r="3" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="30">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+    </row>
+    <row r="4" spans="1:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="30">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="105"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+    </row>
+    <row r="5" spans="1:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="30">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="105"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+    </row>
+    <row r="6" spans="1:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="30">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="105"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+    </row>
+    <row r="7" spans="1:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="30">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="105"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+    </row>
+    <row r="8" spans="1:61" s="29" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="55">
+        <v>6</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="105"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="AM8" s="34"/>
+      <c r="BB8" s="34"/>
+    </row>
+    <row r="9" spans="1:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="54">
+        <v>1</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="106" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="U9" s="39"/>
+    </row>
+    <row r="10" spans="1:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="54">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="106"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+    </row>
+    <row r="11" spans="1:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="56">
+        <v>3</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="106"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="U11" s="27"/>
+    </row>
+    <row r="12" spans="1:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="54">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="106"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+    </row>
+    <row r="13" spans="1:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="54">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="106"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+    </row>
+    <row r="14" spans="1:61" s="29" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="54">
+        <v>6</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="106"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="AM14" s="34"/>
+      <c r="BB14" s="34"/>
+    </row>
+    <row r="15" spans="1:61" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="55">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="106" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+    </row>
+    <row r="16" spans="1:61" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="55">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="106"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+    </row>
+    <row r="17" spans="1:54" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="55">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="106"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+    </row>
+    <row r="18" spans="1:54" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="55">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="106"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="83"/>
+    </row>
+    <row r="19" spans="1:54" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="55">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="106"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+    </row>
+    <row r="20" spans="1:54" s="74" customFormat="1" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="72">
+        <v>6</v>
+      </c>
+      <c r="C20" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="106"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="76"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="83"/>
+      <c r="P20" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM20" s="77"/>
+      <c r="BB20" s="77"/>
+    </row>
+    <row r="21" spans="1:54" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="79">
+        <v>1</v>
+      </c>
+      <c r="C21" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="106" t="s">
+        <v>92</v>
+      </c>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="37"/>
+      <c r="W21" s="37"/>
+      <c r="X21" s="37"/>
+      <c r="Y21" s="37"/>
+    </row>
+    <row r="22" spans="1:54" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="55">
+        <v>2</v>
+      </c>
+      <c r="C22" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="106"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="37"/>
+      <c r="W22" s="37"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="37"/>
+    </row>
+    <row r="23" spans="1:54" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="55">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="106"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="37"/>
+      <c r="W23" s="37"/>
+      <c r="X23" s="37"/>
+      <c r="Y23" s="37"/>
+    </row>
+    <row r="24" spans="1:54" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="55">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="106"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="37"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="37"/>
+      <c r="Y24" s="37"/>
+    </row>
+    <row r="25" spans="1:54" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="55">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="106"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="37"/>
+      <c r="Y25" s="37"/>
+    </row>
+    <row r="26" spans="1:54" s="74" customFormat="1" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="72">
+        <v>6</v>
+      </c>
+      <c r="C26" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="106"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="76"/>
+      <c r="P26" s="82"/>
+      <c r="Q26" s="82"/>
+      <c r="R26" s="82"/>
+      <c r="S26" s="82"/>
+      <c r="T26" s="82"/>
+      <c r="U26" s="82"/>
+      <c r="V26" s="82"/>
+      <c r="W26" s="82"/>
+      <c r="X26" s="82"/>
+      <c r="Y26" s="82"/>
+      <c r="AM26" s="77"/>
+      <c r="BB26" s="77"/>
+    </row>
+    <row r="27" spans="1:54" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="51">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="106" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="Z27" s="59"/>
+      <c r="AA27" s="59"/>
+      <c r="AB27" s="59"/>
+      <c r="AC27" s="59"/>
+      <c r="AD27" s="59"/>
+      <c r="AE27" s="59"/>
+      <c r="AF27" s="59"/>
+      <c r="AG27" s="59"/>
+      <c r="AH27" s="59"/>
+      <c r="AI27" s="59"/>
+      <c r="AJ27" s="59"/>
+      <c r="AK27" s="59"/>
+      <c r="AL27" s="59"/>
+      <c r="AM27" s="59"/>
+    </row>
+    <row r="28" spans="1:54" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="51">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="106"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="Z28" s="37"/>
+      <c r="AA28" s="37"/>
+      <c r="AB28" s="37"/>
+      <c r="AC28" s="37"/>
+      <c r="AD28" s="37"/>
+      <c r="AE28" s="37"/>
+      <c r="AF28" s="37"/>
+      <c r="AG28" s="37"/>
+      <c r="AH28" s="37"/>
+      <c r="AI28" s="37"/>
+      <c r="AJ28" s="37"/>
+      <c r="AK28" s="37"/>
+      <c r="AL28" s="37"/>
+      <c r="AM28" s="37"/>
+    </row>
+    <row r="29" spans="1:54" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="51">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="106"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="Z29" s="37"/>
+      <c r="AA29" s="37"/>
+      <c r="AB29" s="37"/>
+      <c r="AC29" s="37"/>
+      <c r="AD29" s="37"/>
+      <c r="AE29" s="37"/>
+      <c r="AF29" s="37"/>
+      <c r="AG29" s="37"/>
+      <c r="AH29" s="37"/>
+      <c r="AI29" s="37"/>
+      <c r="AJ29" s="37"/>
+      <c r="AK29" s="37"/>
+      <c r="AL29" s="37"/>
+      <c r="AM29" s="37"/>
+    </row>
+    <row r="30" spans="1:54" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="51">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="106"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="Z30" s="37"/>
+      <c r="AA30" s="37"/>
+      <c r="AB30" s="37"/>
+      <c r="AC30" s="37"/>
+      <c r="AD30" s="37"/>
+      <c r="AE30" s="37"/>
+      <c r="AF30" s="37"/>
+      <c r="AG30" s="37"/>
+      <c r="AH30" s="37"/>
+      <c r="AI30" s="37"/>
+      <c r="AJ30" s="37"/>
+      <c r="AK30" s="37"/>
+      <c r="AL30" s="37"/>
+      <c r="AM30" s="37"/>
+    </row>
+    <row r="31" spans="1:54" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="51">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="106"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="Z31" s="37"/>
+      <c r="AA31" s="37"/>
+      <c r="AB31" s="37"/>
+      <c r="AC31" s="37"/>
+      <c r="AD31" s="37"/>
+      <c r="AE31" s="37"/>
+      <c r="AF31" s="37"/>
+      <c r="AG31" s="37"/>
+      <c r="AH31" s="37"/>
+      <c r="AI31" s="37"/>
+      <c r="AJ31" s="37"/>
+      <c r="AK31" s="37"/>
+      <c r="AL31" s="37"/>
+      <c r="AM31" s="37"/>
+    </row>
+    <row r="32" spans="1:54" s="29" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="51">
+        <v>6</v>
+      </c>
+      <c r="C32" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" s="106"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="36"/>
+      <c r="Z32" s="37"/>
+      <c r="AA32" s="37"/>
+      <c r="AB32" s="37"/>
+      <c r="AC32" s="37"/>
+      <c r="AD32" s="37"/>
+      <c r="AE32" s="37"/>
+      <c r="AF32" s="37"/>
+      <c r="AG32" s="37"/>
+      <c r="AH32" s="37"/>
+      <c r="AI32" s="37"/>
+      <c r="AJ32" s="37"/>
+      <c r="AK32" s="37"/>
+      <c r="AL32" s="37"/>
+      <c r="AM32" s="37"/>
+      <c r="BB32" s="34"/>
+    </row>
+    <row r="33" spans="1:69" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="30">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="107" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="AN33" s="37"/>
+      <c r="AO33" s="37"/>
+      <c r="AP33" s="37"/>
+      <c r="AQ33" s="37"/>
+    </row>
+    <row r="34" spans="1:69" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="30">
+        <v>2</v>
+      </c>
+      <c r="E34" s="108"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+    </row>
+    <row r="35" spans="1:69" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="30">
+        <v>3</v>
+      </c>
+      <c r="E35" s="108"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+    </row>
+    <row r="36" spans="1:69" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="30">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="108"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="AN36" s="37"/>
+      <c r="AO36" s="37"/>
+      <c r="AP36" s="37"/>
+      <c r="AQ36" s="37"/>
+    </row>
+    <row r="37" spans="1:69" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="30">
+        <v>5</v>
+      </c>
+      <c r="E37" s="108"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+    </row>
+    <row r="38" spans="1:69" s="29" customFormat="1" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="49">
+        <v>6</v>
+      </c>
+      <c r="C38" s="68"/>
+      <c r="E38" s="109"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="36"/>
+      <c r="AM38" s="34"/>
+      <c r="BB38" s="34"/>
+    </row>
+    <row r="39" spans="1:69" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="30">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="111" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="110" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="AR39" s="59"/>
+      <c r="AS39" s="59"/>
+      <c r="AT39" s="59"/>
+      <c r="AU39" s="59"/>
+      <c r="AV39" s="59"/>
+      <c r="AW39" s="59"/>
+      <c r="AX39" s="59"/>
+      <c r="AY39" s="59"/>
+      <c r="AZ39" s="59"/>
+      <c r="BA39" s="59"/>
+      <c r="BB39" s="59"/>
+    </row>
+    <row r="40" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="30">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="112"/>
+      <c r="E40" s="110"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="41"/>
+      <c r="AR40" s="37"/>
+      <c r="AS40" s="37"/>
+      <c r="AT40" s="37"/>
+      <c r="AU40" s="37"/>
+      <c r="AV40" s="37"/>
+      <c r="AW40" s="37"/>
+      <c r="AX40" s="37"/>
+      <c r="AY40" s="37"/>
+      <c r="AZ40" s="37"/>
+      <c r="BA40" s="37"/>
+      <c r="BB40" s="37"/>
+    </row>
+    <row r="41" spans="1:69" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="30">
+        <v>3</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="112"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="41"/>
+      <c r="AR41" s="37"/>
+      <c r="AS41" s="37"/>
+      <c r="AT41" s="37"/>
+      <c r="AU41" s="37"/>
+      <c r="AV41" s="37"/>
+      <c r="AW41" s="37"/>
+      <c r="AX41" s="37"/>
+      <c r="AY41" s="83"/>
+      <c r="AZ41" s="83"/>
+      <c r="BA41" s="83"/>
+      <c r="BB41" s="83"/>
+      <c r="BC41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:69" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="30">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="112"/>
+      <c r="E42" s="110"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="AR42" s="83"/>
+      <c r="AS42" s="83"/>
+      <c r="AT42" s="83"/>
+      <c r="AU42" s="83"/>
+      <c r="AV42" s="83"/>
+      <c r="AW42" s="83"/>
+      <c r="AX42" s="83"/>
+      <c r="AY42" s="83"/>
+      <c r="AZ42" s="83"/>
+      <c r="BA42" s="83"/>
+      <c r="BB42" s="83"/>
+      <c r="BQ42" s="32"/>
+    </row>
+    <row r="43" spans="1:69" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="30">
+        <v>5</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="112"/>
+      <c r="E43" s="110"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="AR43" s="83"/>
+      <c r="AS43" s="83"/>
+      <c r="AT43" s="83"/>
+      <c r="AU43" s="83"/>
+      <c r="AV43" s="83"/>
+      <c r="AW43" s="83"/>
+      <c r="AX43" s="83"/>
+      <c r="AY43" s="83"/>
+      <c r="AZ43" s="83"/>
+      <c r="BA43" s="83"/>
+      <c r="BB43" s="83"/>
+    </row>
+    <row r="44" spans="1:69" s="29" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="49">
+        <v>6</v>
+      </c>
+      <c r="C44" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="113"/>
+      <c r="E44" s="110"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="36"/>
+      <c r="AM44" s="34"/>
+      <c r="AR44" s="83"/>
+      <c r="AS44" s="83"/>
+      <c r="AT44" s="83"/>
+      <c r="AU44" s="83"/>
+      <c r="AV44" s="83"/>
+      <c r="AW44" s="83"/>
+      <c r="AX44" s="83"/>
+      <c r="AY44" s="83"/>
+      <c r="AZ44" s="83"/>
+      <c r="BA44" s="83"/>
+      <c r="BB44" s="83"/>
+      <c r="BC44" s="28"/>
+      <c r="BD44" s="28"/>
+      <c r="BE44" s="28"/>
+      <c r="BF44" s="28"/>
+      <c r="BG44" s="28"/>
+      <c r="BH44" s="28"/>
+      <c r="BI44" s="28"/>
+    </row>
+    <row r="45" spans="1:69" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" s="41"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="35"/>
+      <c r="AM45" s="33"/>
+      <c r="AQ45"/>
+      <c r="AR45"/>
+      <c r="AS45"/>
+      <c r="AT45"/>
+      <c r="AU45"/>
+      <c r="AV45"/>
+      <c r="AW45"/>
+      <c r="AX45"/>
+      <c r="AY45"/>
+      <c r="AZ45"/>
+      <c r="BA45"/>
+      <c r="BB45"/>
+      <c r="BC45" s="84"/>
+      <c r="BD45" s="84"/>
+      <c r="BE45" s="84"/>
+      <c r="BF45" s="84"/>
+      <c r="BG45" s="84"/>
+      <c r="BH45" s="84"/>
+      <c r="BI45" s="84"/>
+    </row>
+    <row r="46" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="30">
+        <v>1</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="101" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" s="106" t="s">
+        <v>118</v>
+      </c>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="BB46" s="28"/>
+      <c r="BC46" s="84"/>
+      <c r="BD46" s="84"/>
+      <c r="BE46" s="84"/>
+      <c r="BF46" s="84"/>
+      <c r="BG46" s="84"/>
+      <c r="BH46" s="84"/>
+      <c r="BI46" s="84"/>
+    </row>
+    <row r="47" spans="1:69" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="30">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="102"/>
+      <c r="E47" s="106"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="BB47" s="28"/>
+      <c r="BC47" s="84"/>
+      <c r="BD47" s="84"/>
+      <c r="BE47" s="84"/>
+      <c r="BF47" s="84"/>
+      <c r="BG47" s="84"/>
+      <c r="BH47" s="84"/>
+      <c r="BI47" s="84"/>
+    </row>
+    <row r="48" spans="1:69" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="30">
+        <v>3</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="102"/>
+      <c r="E48" s="106"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="41"/>
+      <c r="H48" s="41"/>
+      <c r="BB48" s="28"/>
+      <c r="BC48" s="84"/>
+      <c r="BD48" s="84"/>
+      <c r="BE48" s="84"/>
+      <c r="BF48" s="84"/>
+      <c r="BG48" s="84"/>
+      <c r="BH48" s="84"/>
+      <c r="BI48" s="84"/>
+    </row>
+    <row r="49" spans="1:62" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="30">
+        <v>4</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="102"/>
+      <c r="E49" s="106"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="BB49" s="28"/>
+      <c r="BC49" s="84"/>
+      <c r="BD49" s="84"/>
+      <c r="BE49" s="84"/>
+      <c r="BF49" s="84"/>
+      <c r="BG49" s="84"/>
+      <c r="BH49" s="84"/>
+      <c r="BI49" s="84"/>
+    </row>
+    <row r="50" spans="1:62" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="30">
+        <v>5</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="102"/>
+      <c r="E50" s="106"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="BB50" s="28"/>
+      <c r="BC50" s="84"/>
+      <c r="BD50" s="84"/>
+      <c r="BE50" s="84"/>
+      <c r="BF50" s="84"/>
+      <c r="BG50" s="84"/>
+      <c r="BH50" s="84"/>
+      <c r="BI50" s="84"/>
+    </row>
+    <row r="51" spans="1:62" s="29" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="30">
+        <v>6</v>
+      </c>
+      <c r="C51" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="103"/>
+      <c r="E51" s="106"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="36"/>
+      <c r="AM51" s="34"/>
+      <c r="BC51" s="84"/>
+      <c r="BD51" s="84"/>
+      <c r="BE51" s="84"/>
+      <c r="BF51" s="84"/>
+      <c r="BG51" s="84"/>
+      <c r="BH51" s="84"/>
+      <c r="BI51" s="84"/>
+      <c r="BJ51" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A52" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="30">
+        <v>1</v>
+      </c>
+      <c r="E52" s="104" t="s">
+        <v>73</v>
+      </c>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+    </row>
+    <row r="53" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A53" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="30">
+        <v>2</v>
+      </c>
+      <c r="E53" s="104"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+    </row>
+    <row r="54" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A54" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="30">
+        <v>3</v>
+      </c>
+      <c r="E54" s="104"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="41"/>
+    </row>
+    <row r="55" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A55" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="30">
+        <v>4</v>
+      </c>
+      <c r="E55" s="104"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="41"/>
+      <c r="H55" s="41"/>
+    </row>
+    <row r="56" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A56" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="30">
+        <v>5</v>
+      </c>
+      <c r="E56" s="104"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
+    </row>
+    <row r="57" spans="1:62" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="49">
+        <v>6</v>
+      </c>
+      <c r="C57" s="68"/>
+      <c r="E57" s="104"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="42"/>
+      <c r="I57" s="36"/>
+      <c r="AM57" s="34"/>
+      <c r="BB57" s="34"/>
+    </row>
+    <row r="58" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A58" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="30">
+        <v>1</v>
+      </c>
+      <c r="E58" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" s="41"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="41"/>
+    </row>
+    <row r="59" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A59" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" s="30">
+        <v>2</v>
+      </c>
+      <c r="E59" s="104"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="41"/>
+    </row>
+    <row r="60" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A60" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="30">
+        <v>3</v>
+      </c>
+      <c r="E60" s="104"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="41"/>
+    </row>
+    <row r="61" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A61" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="30">
+        <v>4</v>
+      </c>
+      <c r="E61" s="104"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="41"/>
+    </row>
+    <row r="62" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A62" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="30">
+        <v>5</v>
+      </c>
+      <c r="E62" s="104"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="41"/>
+    </row>
+    <row r="63" spans="1:62" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="30">
+        <v>6</v>
+      </c>
+      <c r="C63" s="68"/>
+      <c r="E63" s="104"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="36"/>
+      <c r="AM63" s="34"/>
+      <c r="BB63" s="34"/>
+    </row>
+    <row r="64" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A64" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="30"/>
+      <c r="E64" s="104" t="s">
+        <v>75</v>
+      </c>
+      <c r="F64" s="41"/>
+      <c r="G64" s="41"/>
+      <c r="H64" s="41"/>
+    </row>
+    <row r="65" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A65" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="30"/>
+      <c r="E65" s="104"/>
+      <c r="F65" s="41"/>
+      <c r="G65" s="41"/>
+      <c r="H65" s="41"/>
+    </row>
+    <row r="66" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A66" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="30"/>
+      <c r="E66" s="104"/>
+      <c r="F66" s="41"/>
+      <c r="G66" s="41"/>
+      <c r="H66" s="41"/>
+    </row>
+    <row r="67" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A67" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="30"/>
+      <c r="E67" s="104"/>
+      <c r="F67" s="41"/>
+      <c r="G67" s="41"/>
+      <c r="H67" s="41"/>
+    </row>
+    <row r="68" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A68" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="30"/>
+      <c r="E68" s="104"/>
+      <c r="F68" s="41"/>
+      <c r="G68" s="41"/>
+      <c r="H68" s="41"/>
+    </row>
+    <row r="69" spans="1:54" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="31"/>
+      <c r="C69" s="68"/>
+      <c r="E69" s="104"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
+      <c r="H69" s="42"/>
+      <c r="I69" s="36"/>
+      <c r="AM69" s="34"/>
+      <c r="BB69" s="34"/>
+    </row>
+    <row r="70" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A70" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="30"/>
+      <c r="E70" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="F70" s="41"/>
+      <c r="G70" s="41"/>
+      <c r="H70" s="41"/>
+    </row>
+    <row r="71" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A71" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="30"/>
+      <c r="E71" s="104"/>
+      <c r="F71" s="41"/>
+      <c r="G71" s="41"/>
+      <c r="H71" s="41"/>
+    </row>
+    <row r="72" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A72" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" s="30"/>
+      <c r="E72" s="104"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="41"/>
+      <c r="H72" s="41"/>
+    </row>
+    <row r="73" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A73" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="30"/>
+      <c r="E73" s="104"/>
+      <c r="F73" s="41"/>
+      <c r="G73" s="41"/>
+      <c r="H73" s="41"/>
+    </row>
+    <row r="74" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A74" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="30"/>
+      <c r="E74" s="104"/>
+      <c r="F74" s="41"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="41"/>
+    </row>
+    <row r="75" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="31"/>
+      <c r="C75" s="68"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="104"/>
+      <c r="F75" s="41"/>
+      <c r="G75" s="41"/>
+      <c r="H75" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="E70:E75"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="E39:E44"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="E46:E51"/>
+    <mergeCell ref="E52:E57"/>
+    <mergeCell ref="E58:E63"/>
+    <mergeCell ref="J2:AM2"/>
+    <mergeCell ref="AN2:BB2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="D46:D51"/>
+    <mergeCell ref="E64:E69"/>
+    <mergeCell ref="D39:D44"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1604,17 +4217,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1656,12 +4269,12 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="22" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1692,7 +4305,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
         <v>46</v>
@@ -1715,7 +4328,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Update report, plan, test files
</commit_message>
<xml_diff>
--- a/document/Bảng phân công.xlsx
+++ b/document/Bảng phân công.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="130">
   <si>
     <t>Nhật</t>
   </si>
@@ -372,9 +372,6 @@
   </si>
   <si>
     <t>Thiết kế giai đoạn 2</t>
-  </si>
-  <si>
-    <t>Chưa update document</t>
   </si>
   <si>
     <t>QL tài khoản</t>
@@ -388,9 +385,6 @@
   <si>
     <t xml:space="preserve">Design UI(adobe and code Frontend), Detail UI, SRS
 </t>
-  </si>
-  <si>
-    <t>Đang tiến hành</t>
   </si>
   <si>
     <t>Code logic các chức năng giai đoạn 2</t>
@@ -1478,6 +1472,24 @@
     <xf numFmtId="16" fontId="4" fillId="5" borderId="16" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1521,24 +1533,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
@@ -2543,10 +2537,10 @@
   <dimension ref="A1:CW75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AX41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="CF46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CC55" sqref="CC55"/>
+      <selection pane="bottomRight" activeCell="BI62" sqref="BI62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2824,110 +2818,110 @@
       <c r="E2" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="107" t="s">
+      <c r="F2" s="113" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="104" t="s">
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="105"/>
-      <c r="S2" s="105"/>
-      <c r="T2" s="105"/>
-      <c r="U2" s="105"/>
-      <c r="V2" s="105"/>
-      <c r="W2" s="105"/>
-      <c r="X2" s="105"/>
-      <c r="Y2" s="105"/>
-      <c r="Z2" s="105"/>
-      <c r="AA2" s="105"/>
-      <c r="AB2" s="105"/>
-      <c r="AC2" s="105"/>
-      <c r="AD2" s="105"/>
-      <c r="AE2" s="105"/>
-      <c r="AF2" s="105"/>
-      <c r="AG2" s="105"/>
-      <c r="AH2" s="105"/>
-      <c r="AI2" s="105"/>
-      <c r="AJ2" s="105"/>
-      <c r="AK2" s="105"/>
-      <c r="AL2" s="105"/>
-      <c r="AM2" s="106"/>
-      <c r="AN2" s="96" t="s">
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="111"/>
+      <c r="AA2" s="111"/>
+      <c r="AB2" s="111"/>
+      <c r="AC2" s="111"/>
+      <c r="AD2" s="111"/>
+      <c r="AE2" s="111"/>
+      <c r="AF2" s="111"/>
+      <c r="AG2" s="111"/>
+      <c r="AH2" s="111"/>
+      <c r="AI2" s="111"/>
+      <c r="AJ2" s="111"/>
+      <c r="AK2" s="111"/>
+      <c r="AL2" s="111"/>
+      <c r="AM2" s="112"/>
+      <c r="AN2" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="AO2" s="97"/>
-      <c r="AP2" s="97"/>
-      <c r="AQ2" s="97"/>
-      <c r="AR2" s="97"/>
-      <c r="AS2" s="97"/>
-      <c r="AT2" s="97"/>
-      <c r="AU2" s="97"/>
-      <c r="AV2" s="97"/>
-      <c r="AW2" s="97"/>
-      <c r="AX2" s="97"/>
-      <c r="AY2" s="97"/>
-      <c r="AZ2" s="97"/>
-      <c r="BA2" s="97"/>
-      <c r="BB2" s="97"/>
-      <c r="BC2" s="97"/>
-      <c r="BD2" s="97"/>
-      <c r="BE2" s="97"/>
-      <c r="BF2" s="97"/>
-      <c r="BG2" s="97"/>
-      <c r="BH2" s="97"/>
-      <c r="BI2" s="97"/>
-      <c r="BJ2" s="97"/>
-      <c r="BK2" s="97"/>
-      <c r="BL2" s="97"/>
-      <c r="BM2" s="97"/>
-      <c r="BN2" s="97"/>
-      <c r="BO2" s="97"/>
-      <c r="BP2" s="97"/>
-      <c r="BQ2" s="97"/>
-      <c r="BR2" s="97"/>
-      <c r="BS2" s="96" t="s">
-        <v>124</v>
-      </c>
-      <c r="BT2" s="97"/>
-      <c r="BU2" s="97"/>
-      <c r="BV2" s="97"/>
-      <c r="BW2" s="97"/>
-      <c r="BX2" s="97"/>
-      <c r="BY2" s="97"/>
-      <c r="BZ2" s="97"/>
-      <c r="CA2" s="97"/>
-      <c r="CB2" s="97"/>
-      <c r="CC2" s="97"/>
-      <c r="CD2" s="97"/>
-      <c r="CE2" s="97"/>
-      <c r="CF2" s="97"/>
-      <c r="CG2" s="97"/>
-      <c r="CH2" s="97"/>
-      <c r="CI2" s="97"/>
-      <c r="CJ2" s="97"/>
-      <c r="CK2" s="97"/>
-      <c r="CL2" s="97"/>
-      <c r="CM2" s="97"/>
-      <c r="CN2" s="97"/>
-      <c r="CO2" s="97"/>
-      <c r="CP2" s="97"/>
-      <c r="CQ2" s="97"/>
-      <c r="CR2" s="97"/>
-      <c r="CS2" s="97"/>
-      <c r="CT2" s="97"/>
-      <c r="CU2" s="97"/>
-      <c r="CV2" s="97"/>
-      <c r="CW2" s="97"/>
+      <c r="AO2" s="103"/>
+      <c r="AP2" s="103"/>
+      <c r="AQ2" s="103"/>
+      <c r="AR2" s="103"/>
+      <c r="AS2" s="103"/>
+      <c r="AT2" s="103"/>
+      <c r="AU2" s="103"/>
+      <c r="AV2" s="103"/>
+      <c r="AW2" s="103"/>
+      <c r="AX2" s="103"/>
+      <c r="AY2" s="103"/>
+      <c r="AZ2" s="103"/>
+      <c r="BA2" s="103"/>
+      <c r="BB2" s="103"/>
+      <c r="BC2" s="103"/>
+      <c r="BD2" s="103"/>
+      <c r="BE2" s="103"/>
+      <c r="BF2" s="103"/>
+      <c r="BG2" s="103"/>
+      <c r="BH2" s="103"/>
+      <c r="BI2" s="103"/>
+      <c r="BJ2" s="103"/>
+      <c r="BK2" s="103"/>
+      <c r="BL2" s="103"/>
+      <c r="BM2" s="103"/>
+      <c r="BN2" s="103"/>
+      <c r="BO2" s="103"/>
+      <c r="BP2" s="103"/>
+      <c r="BQ2" s="103"/>
+      <c r="BR2" s="103"/>
+      <c r="BS2" s="102" t="s">
+        <v>122</v>
+      </c>
+      <c r="BT2" s="103"/>
+      <c r="BU2" s="103"/>
+      <c r="BV2" s="103"/>
+      <c r="BW2" s="103"/>
+      <c r="BX2" s="103"/>
+      <c r="BY2" s="103"/>
+      <c r="BZ2" s="103"/>
+      <c r="CA2" s="103"/>
+      <c r="CB2" s="103"/>
+      <c r="CC2" s="103"/>
+      <c r="CD2" s="103"/>
+      <c r="CE2" s="103"/>
+      <c r="CF2" s="103"/>
+      <c r="CG2" s="103"/>
+      <c r="CH2" s="103"/>
+      <c r="CI2" s="103"/>
+      <c r="CJ2" s="103"/>
+      <c r="CK2" s="103"/>
+      <c r="CL2" s="103"/>
+      <c r="CM2" s="103"/>
+      <c r="CN2" s="103"/>
+      <c r="CO2" s="103"/>
+      <c r="CP2" s="103"/>
+      <c r="CQ2" s="103"/>
+      <c r="CR2" s="103"/>
+      <c r="CS2" s="103"/>
+      <c r="CT2" s="103"/>
+      <c r="CU2" s="103"/>
+      <c r="CV2" s="103"/>
+      <c r="CW2" s="103"/>
     </row>
     <row r="3" spans="1:101" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="30">
@@ -2936,7 +2930,7 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="109" t="s">
         <v>75</v>
       </c>
       <c r="D3" s="57" t="s">
@@ -2954,7 +2948,7 @@
       <c r="B4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="109"/>
       <c r="D4" s="57" t="s">
         <v>69</v>
       </c>
@@ -2970,7 +2964,7 @@
       <c r="B5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="103"/>
+      <c r="C5" s="109"/>
       <c r="D5" s="57" t="s">
         <v>3</v>
       </c>
@@ -2986,7 +2980,7 @@
       <c r="B6" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="103"/>
+      <c r="C6" s="109"/>
       <c r="D6" s="57" t="s">
         <v>5</v>
       </c>
@@ -3002,7 +2996,7 @@
       <c r="B7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="103"/>
+      <c r="C7" s="109"/>
       <c r="D7" s="57" t="s">
         <v>4</v>
       </c>
@@ -3018,7 +3012,7 @@
       <c r="B8" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="103"/>
+      <c r="C8" s="109"/>
       <c r="D8" s="57" t="s">
         <v>1</v>
       </c>
@@ -3042,7 +3036,7 @@
       <c r="B9" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="102" t="s">
+      <c r="C9" s="108" t="s">
         <v>81</v>
       </c>
       <c r="D9" s="50" t="s">
@@ -3067,7 +3061,7 @@
       <c r="B10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="102"/>
+      <c r="C10" s="108"/>
       <c r="D10" s="50" t="s">
         <v>69</v>
       </c>
@@ -3086,7 +3080,7 @@
       <c r="B11" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="102"/>
+      <c r="C11" s="108"/>
       <c r="D11" s="50" t="s">
         <v>3</v>
       </c>
@@ -3106,7 +3100,7 @@
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="102"/>
+      <c r="C12" s="108"/>
       <c r="D12" s="50" t="s">
         <v>5</v>
       </c>
@@ -3125,7 +3119,7 @@
       <c r="B13" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="102"/>
+      <c r="C13" s="108"/>
       <c r="D13" s="50" t="s">
         <v>4</v>
       </c>
@@ -3144,7 +3138,7 @@
       <c r="B14" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="102"/>
+      <c r="C14" s="108"/>
       <c r="D14" s="50" t="s">
         <v>1</v>
       </c>
@@ -3168,7 +3162,7 @@
       <c r="B15" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="102" t="s">
+      <c r="C15" s="108" t="s">
         <v>103</v>
       </c>
       <c r="D15" s="57" t="s">
@@ -3186,7 +3180,7 @@
       <c r="B16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="102"/>
+      <c r="C16" s="108"/>
       <c r="D16" s="57" t="s">
         <v>69</v>
       </c>
@@ -3202,7 +3196,7 @@
       <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="102"/>
+      <c r="C17" s="108"/>
       <c r="D17" s="57" t="s">
         <v>3</v>
       </c>
@@ -3221,7 +3215,7 @@
       <c r="B18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="102"/>
+      <c r="C18" s="108"/>
       <c r="D18" s="57" t="s">
         <v>5</v>
       </c>
@@ -3237,7 +3231,7 @@
       <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="102"/>
+      <c r="C19" s="108"/>
       <c r="D19" s="57" t="s">
         <v>4</v>
       </c>
@@ -3253,7 +3247,7 @@
       <c r="B20" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="102"/>
+      <c r="C20" s="108"/>
       <c r="D20" s="80" t="s">
         <v>1</v>
       </c>
@@ -3275,7 +3269,7 @@
       <c r="B21" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="102" t="s">
+      <c r="C21" s="108" t="s">
         <v>90</v>
       </c>
       <c r="D21" s="78" t="s">
@@ -3299,7 +3293,7 @@
       <c r="B22" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="102"/>
+      <c r="C22" s="108"/>
       <c r="D22" s="66" t="s">
         <v>69</v>
       </c>
@@ -3321,7 +3315,7 @@
       <c r="B23" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="102"/>
+      <c r="C23" s="108"/>
       <c r="D23" s="66" t="s">
         <v>3</v>
       </c>
@@ -3343,7 +3337,7 @@
       <c r="B24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="102"/>
+      <c r="C24" s="108"/>
       <c r="D24" s="66" t="s">
         <v>5</v>
       </c>
@@ -3365,7 +3359,7 @@
       <c r="B25" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="102"/>
+      <c r="C25" s="108"/>
       <c r="D25" s="66" t="s">
         <v>4</v>
       </c>
@@ -3387,7 +3381,7 @@
       <c r="B26" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="102"/>
+      <c r="C26" s="108"/>
       <c r="D26" s="71" t="s">
         <v>1</v>
       </c>
@@ -3415,7 +3409,7 @@
       <c r="B27" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="102" t="s">
+      <c r="C27" s="108" t="s">
         <v>97</v>
       </c>
       <c r="D27" s="52" t="s">
@@ -3446,7 +3440,7 @@
       <c r="B28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="102"/>
+      <c r="C28" s="108"/>
       <c r="D28" s="52" t="s">
         <v>69</v>
       </c>
@@ -3475,7 +3469,7 @@
       <c r="B29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="102"/>
+      <c r="C29" s="108"/>
       <c r="D29" s="52" t="s">
         <v>3</v>
       </c>
@@ -3504,7 +3498,7 @@
       <c r="B30" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="102"/>
+      <c r="C30" s="108"/>
       <c r="D30" s="52" t="s">
         <v>5</v>
       </c>
@@ -3533,7 +3527,7 @@
       <c r="B31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="102"/>
+      <c r="C31" s="108"/>
       <c r="D31" s="52" t="s">
         <v>4</v>
       </c>
@@ -3562,7 +3556,7 @@
       <c r="B32" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="102"/>
+      <c r="C32" s="108"/>
       <c r="D32" s="53" t="s">
         <v>1</v>
       </c>
@@ -3593,7 +3587,7 @@
       <c r="B33" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="98" t="s">
+      <c r="C33" s="104" t="s">
         <v>101</v>
       </c>
       <c r="D33" s="58" t="s">
@@ -3611,7 +3605,7 @@
       <c r="A34" s="30">
         <v>2</v>
       </c>
-      <c r="C34" s="99"/>
+      <c r="C34" s="105"/>
       <c r="D34" s="58" t="s">
         <v>69</v>
       </c>
@@ -3623,7 +3617,7 @@
       <c r="A35" s="30">
         <v>3</v>
       </c>
-      <c r="C35" s="99"/>
+      <c r="C35" s="105"/>
       <c r="D35" s="58" t="s">
         <v>3</v>
       </c>
@@ -3638,7 +3632,7 @@
       <c r="B36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="99"/>
+      <c r="C36" s="105"/>
       <c r="D36" s="58" t="s">
         <v>5</v>
       </c>
@@ -3654,7 +3648,7 @@
       <c r="A37" s="30">
         <v>5</v>
       </c>
-      <c r="C37" s="99"/>
+      <c r="C37" s="105"/>
       <c r="D37" s="58" t="s">
         <v>4</v>
       </c>
@@ -3667,7 +3661,7 @@
         <v>6</v>
       </c>
       <c r="B38" s="68"/>
-      <c r="C38" s="100"/>
+      <c r="C38" s="106"/>
       <c r="D38" s="58" t="s">
         <v>1</v>
       </c>
@@ -3685,13 +3679,13 @@
       <c r="B39" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="101" t="s">
+      <c r="C39" s="107" t="s">
         <v>114</v>
       </c>
       <c r="D39" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E39" s="113" t="s">
+      <c r="E39" s="98" t="s">
         <v>115</v>
       </c>
       <c r="F39" s="41"/>
@@ -3716,11 +3710,11 @@
       <c r="B40" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C40" s="101"/>
+      <c r="C40" s="107"/>
       <c r="D40" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="114"/>
+      <c r="E40" s="99"/>
       <c r="F40" s="41"/>
       <c r="G40" s="41"/>
       <c r="H40" s="41"/>
@@ -3736,18 +3730,18 @@
       <c r="BA40" s="37"/>
       <c r="BB40" s="37"/>
     </row>
-    <row r="41" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>3</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="101"/>
+      <c r="C41" s="107"/>
       <c r="D41" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="114"/>
+      <c r="E41" s="99"/>
       <c r="F41" s="41"/>
       <c r="G41" s="41"/>
       <c r="H41" s="41"/>
@@ -3758,97 +3752,94 @@
       <c r="AV41" s="37"/>
       <c r="AW41" s="37"/>
       <c r="AX41" s="37"/>
-      <c r="AY41" s="83"/>
-      <c r="AZ41" s="83"/>
-      <c r="BA41" s="83"/>
-      <c r="BB41" s="83"/>
-      <c r="BC41" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY41" s="37"/>
+      <c r="AZ41" s="37"/>
+      <c r="BA41" s="37"/>
+      <c r="BB41" s="37"/>
+    </row>
+    <row r="42" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>4</v>
       </c>
       <c r="B42" t="s">
         <v>112</v>
       </c>
-      <c r="C42" s="101"/>
+      <c r="C42" s="107"/>
       <c r="D42" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="114"/>
+      <c r="E42" s="99"/>
       <c r="F42" s="41"/>
       <c r="G42" s="41"/>
       <c r="H42" s="41"/>
-      <c r="AR42" s="83"/>
-      <c r="AS42" s="83"/>
-      <c r="AT42" s="83"/>
-      <c r="AU42" s="83"/>
-      <c r="AV42" s="83"/>
-      <c r="AW42" s="83"/>
-      <c r="AX42" s="83"/>
-      <c r="AY42" s="83"/>
-      <c r="AZ42" s="83"/>
-      <c r="BA42" s="83"/>
-      <c r="BB42" s="83"/>
+      <c r="AR42" s="37"/>
+      <c r="AS42" s="37"/>
+      <c r="AT42" s="37"/>
+      <c r="AU42" s="37"/>
+      <c r="AV42" s="37"/>
+      <c r="AW42" s="37"/>
+      <c r="AX42" s="37"/>
+      <c r="AY42" s="37"/>
+      <c r="AZ42" s="37"/>
+      <c r="BA42" s="37"/>
+      <c r="BB42" s="37"/>
       <c r="BQ42" s="32"/>
     </row>
-    <row r="43" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="101"/>
+      <c r="C43" s="107"/>
       <c r="D43" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="114"/>
+      <c r="E43" s="99"/>
       <c r="F43" s="41"/>
       <c r="G43" s="41"/>
       <c r="H43" s="41"/>
-      <c r="AR43" s="83"/>
-      <c r="AS43" s="83"/>
-      <c r="AT43" s="83"/>
-      <c r="AU43" s="83"/>
-      <c r="AV43" s="83"/>
-      <c r="AW43" s="83"/>
-      <c r="AX43" s="83"/>
-      <c r="AY43" s="83"/>
-      <c r="AZ43" s="83"/>
-      <c r="BA43" s="83"/>
-      <c r="BB43" s="83"/>
-    </row>
-    <row r="44" spans="1:74" s="29" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AR43" s="37"/>
+      <c r="AS43" s="37"/>
+      <c r="AT43" s="37"/>
+      <c r="AU43" s="37"/>
+      <c r="AV43" s="37"/>
+      <c r="AW43" s="37"/>
+      <c r="AX43" s="37"/>
+      <c r="AY43" s="37"/>
+      <c r="AZ43" s="37"/>
+      <c r="BA43" s="37"/>
+      <c r="BB43" s="37"/>
+    </row>
+    <row r="44" spans="1:74" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="49">
         <v>6</v>
       </c>
       <c r="B44" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="101"/>
+      <c r="C44" s="107"/>
       <c r="D44" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E44" s="115"/>
+      <c r="E44" s="100"/>
       <c r="F44" s="42"/>
       <c r="G44" s="42"/>
       <c r="H44" s="42"/>
       <c r="I44" s="36"/>
       <c r="AM44" s="34"/>
-      <c r="AR44" s="83"/>
-      <c r="AS44" s="83"/>
-      <c r="AT44" s="83"/>
-      <c r="AU44" s="83"/>
-      <c r="AV44" s="83"/>
-      <c r="AW44" s="83"/>
-      <c r="AX44" s="83"/>
-      <c r="AY44" s="83"/>
-      <c r="AZ44" s="83"/>
-      <c r="BA44" s="83"/>
-      <c r="BB44" s="83"/>
+      <c r="AR44" s="37"/>
+      <c r="AS44" s="37"/>
+      <c r="AT44" s="37"/>
+      <c r="AU44" s="37"/>
+      <c r="AV44" s="37"/>
+      <c r="AW44" s="37"/>
+      <c r="AX44" s="37"/>
+      <c r="AY44" s="37"/>
+      <c r="AZ44" s="37"/>
+      <c r="BA44" s="37"/>
+      <c r="BB44" s="37"/>
     </row>
     <row r="45" spans="1:74" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="85"/>
@@ -3883,14 +3874,14 @@
       <c r="B46" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="102" t="s">
+      <c r="C46" s="108" t="s">
         <v>116</v>
       </c>
       <c r="D46" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E46" s="110" t="s">
-        <v>121</v>
+      <c r="E46" s="95" t="s">
+        <v>120</v>
       </c>
       <c r="F46" s="41"/>
       <c r="G46" s="41"/>
@@ -3916,13 +3907,13 @@
         <v>2</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C47" s="102"/>
+        <v>117</v>
+      </c>
+      <c r="C47" s="108"/>
       <c r="D47" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="111"/>
+      <c r="E47" s="96"/>
       <c r="F47" s="41"/>
       <c r="G47" s="41"/>
       <c r="H47" s="41"/>
@@ -3942,11 +3933,11 @@
       <c r="B48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="102"/>
+      <c r="C48" s="108"/>
       <c r="D48" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="111"/>
+      <c r="E48" s="96"/>
       <c r="F48" s="41"/>
       <c r="G48" s="41"/>
       <c r="H48" s="41"/>
@@ -3964,37 +3955,37 @@
         <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C49" s="102"/>
+        <v>119</v>
+      </c>
+      <c r="C49" s="108"/>
       <c r="D49" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E49" s="111"/>
+      <c r="E49" s="96"/>
       <c r="F49" s="41"/>
       <c r="G49" s="41"/>
       <c r="H49" s="41"/>
       <c r="BB49" s="28"/>
-      <c r="BC49" s="84"/>
-      <c r="BD49" s="84"/>
-      <c r="BE49" s="84"/>
-      <c r="BF49" s="84"/>
-      <c r="BG49" s="84"/>
-      <c r="BH49" s="84"/>
-      <c r="BI49" s="84"/>
+      <c r="BC49" s="37"/>
+      <c r="BD49" s="37"/>
+      <c r="BE49" s="37"/>
+      <c r="BF49" s="37"/>
+      <c r="BG49" s="37"/>
+      <c r="BH49" s="37"/>
+      <c r="BI49" s="37"/>
     </row>
     <row r="50" spans="1:75" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>5</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C50" s="102"/>
+        <v>118</v>
+      </c>
+      <c r="C50" s="108"/>
       <c r="D50" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="111"/>
+      <c r="E50" s="96"/>
       <c r="F50" s="41"/>
       <c r="G50" s="41"/>
       <c r="H50" s="41"/>
@@ -4014,26 +4005,23 @@
       <c r="B51" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="102"/>
+      <c r="C51" s="108"/>
       <c r="D51" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E51" s="112"/>
+      <c r="E51" s="97"/>
       <c r="F51" s="42"/>
       <c r="G51" s="42"/>
       <c r="H51" s="42"/>
       <c r="I51" s="36"/>
       <c r="AM51" s="34"/>
-      <c r="BC51" s="84"/>
-      <c r="BD51" s="84"/>
-      <c r="BE51" s="84"/>
-      <c r="BF51" s="84"/>
-      <c r="BG51" s="84"/>
-      <c r="BH51" s="84"/>
-      <c r="BI51" s="84"/>
-      <c r="BJ51" s="29" t="s">
-        <v>122</v>
-      </c>
+      <c r="BC51" s="37"/>
+      <c r="BD51" s="37"/>
+      <c r="BE51" s="37"/>
+      <c r="BF51" s="37"/>
+      <c r="BG51" s="37"/>
+      <c r="BH51" s="37"/>
+      <c r="BI51" s="37"/>
     </row>
     <row r="52" spans="1:75" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
@@ -4042,8 +4030,8 @@
       <c r="B52" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C52" s="101" t="s">
-        <v>123</v>
+      <c r="C52" s="107" t="s">
+        <v>121</v>
       </c>
       <c r="D52" s="30" t="s">
         <v>0</v>
@@ -4064,9 +4052,9 @@
         <v>2</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" s="101"/>
+        <v>117</v>
+      </c>
+      <c r="C53" s="107"/>
       <c r="D53" s="30" t="s">
         <v>69</v>
       </c>
@@ -4088,7 +4076,7 @@
       <c r="B54" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="101"/>
+      <c r="C54" s="107"/>
       <c r="D54" s="30" t="s">
         <v>3</v>
       </c>
@@ -4108,9 +4096,9 @@
         <v>4</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C55" s="101"/>
+        <v>119</v>
+      </c>
+      <c r="C55" s="107"/>
       <c r="D55" s="30" t="s">
         <v>5</v>
       </c>
@@ -4130,9 +4118,9 @@
         <v>5</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C56" s="101"/>
+        <v>118</v>
+      </c>
+      <c r="C56" s="107"/>
       <c r="D56" s="30" t="s">
         <v>4</v>
       </c>
@@ -4154,7 +4142,7 @@
       <c r="B57" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="101"/>
+      <c r="C57" s="107"/>
       <c r="D57" s="31" t="s">
         <v>1</v>
       </c>
@@ -4177,10 +4165,10 @@
         <v>1</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C58" s="102" t="s">
-        <v>125</v>
+        <v>127</v>
+      </c>
+      <c r="C58" s="108" t="s">
+        <v>123</v>
       </c>
       <c r="D58" s="30" t="s">
         <v>0</v>
@@ -4201,53 +4189,53 @@
         <v>2</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C59" s="102"/>
+        <v>124</v>
+      </c>
+      <c r="C59" s="108"/>
       <c r="D59" s="30" t="s">
         <v>69</v>
       </c>
       <c r="F59" s="41"/>
       <c r="G59" s="41"/>
       <c r="H59" s="41"/>
-      <c r="BQ59" s="84"/>
-      <c r="BR59" s="84"/>
-      <c r="BS59" s="84"/>
-      <c r="BT59" s="84"/>
-      <c r="BU59" s="84"/>
-      <c r="BV59" s="84"/>
-      <c r="BW59" s="84"/>
+      <c r="BQ59" s="37"/>
+      <c r="BR59" s="37"/>
+      <c r="BS59" s="37"/>
+      <c r="BT59" s="37"/>
+      <c r="BU59" s="37"/>
+      <c r="BV59" s="37"/>
+      <c r="BW59" s="37"/>
     </row>
     <row r="60" spans="1:75" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>3</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C60" s="102"/>
+        <v>125</v>
+      </c>
+      <c r="C60" s="108"/>
       <c r="D60" s="30" t="s">
         <v>3</v>
       </c>
       <c r="F60" s="41"/>
       <c r="G60" s="41"/>
       <c r="H60" s="41"/>
-      <c r="BQ60" s="84"/>
-      <c r="BR60" s="84"/>
-      <c r="BS60" s="84"/>
-      <c r="BT60" s="84"/>
-      <c r="BU60" s="84"/>
-      <c r="BV60" s="84"/>
-      <c r="BW60" s="84"/>
+      <c r="BQ60" s="37"/>
+      <c r="BR60" s="37"/>
+      <c r="BS60" s="37"/>
+      <c r="BT60" s="37"/>
+      <c r="BU60" s="37"/>
+      <c r="BV60" s="37"/>
+      <c r="BW60" s="37"/>
     </row>
     <row r="61" spans="1:75" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>4</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C61" s="102"/>
+        <v>128</v>
+      </c>
+      <c r="C61" s="108"/>
       <c r="D61" s="30" t="s">
         <v>5</v>
       </c>
@@ -4267,31 +4255,31 @@
         <v>5</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" s="102"/>
+        <v>126</v>
+      </c>
+      <c r="C62" s="108"/>
       <c r="D62" s="30" t="s">
         <v>4</v>
       </c>
       <c r="F62" s="41"/>
       <c r="G62" s="41"/>
       <c r="H62" s="41"/>
-      <c r="BQ62" s="84"/>
-      <c r="BR62" s="84"/>
-      <c r="BS62" s="84"/>
-      <c r="BT62" s="84"/>
-      <c r="BU62" s="84"/>
-      <c r="BV62" s="84"/>
-      <c r="BW62" s="84"/>
+      <c r="BQ62" s="37"/>
+      <c r="BR62" s="37"/>
+      <c r="BS62" s="37"/>
+      <c r="BT62" s="37"/>
+      <c r="BU62" s="37"/>
+      <c r="BV62" s="37"/>
+      <c r="BW62" s="37"/>
     </row>
     <row r="63" spans="1:75" s="29" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>6</v>
       </c>
       <c r="B63" s="68" t="s">
-        <v>131</v>
-      </c>
-      <c r="C63" s="102"/>
+        <v>129</v>
+      </c>
+      <c r="C63" s="108"/>
       <c r="D63" s="31" t="s">
         <v>1</v>
       </c>
@@ -4311,7 +4299,7 @@
     </row>
     <row r="64" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A64" s="30"/>
-      <c r="C64" s="95" t="s">
+      <c r="C64" s="101" t="s">
         <v>73</v>
       </c>
       <c r="D64" s="30" t="s">
@@ -4323,7 +4311,7 @@
     </row>
     <row r="65" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A65" s="30"/>
-      <c r="C65" s="95"/>
+      <c r="C65" s="101"/>
       <c r="D65" s="30" t="s">
         <v>69</v>
       </c>
@@ -4333,7 +4321,7 @@
     </row>
     <row r="66" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A66" s="30"/>
-      <c r="C66" s="95"/>
+      <c r="C66" s="101"/>
       <c r="D66" s="30" t="s">
         <v>3</v>
       </c>
@@ -4343,7 +4331,7 @@
     </row>
     <row r="67" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A67" s="30"/>
-      <c r="C67" s="95"/>
+      <c r="C67" s="101"/>
       <c r="D67" s="30" t="s">
         <v>5</v>
       </c>
@@ -4353,7 +4341,7 @@
     </row>
     <row r="68" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A68" s="30"/>
-      <c r="C68" s="95"/>
+      <c r="C68" s="101"/>
       <c r="D68" s="30" t="s">
         <v>4</v>
       </c>
@@ -4364,7 +4352,7 @@
     <row r="69" spans="1:54" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="31"/>
       <c r="B69" s="68"/>
-      <c r="C69" s="95"/>
+      <c r="C69" s="101"/>
       <c r="D69" s="31" t="s">
         <v>1</v>
       </c>
@@ -4377,7 +4365,7 @@
     </row>
     <row r="70" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A70" s="30"/>
-      <c r="C70" s="95" t="s">
+      <c r="C70" s="101" t="s">
         <v>74</v>
       </c>
       <c r="D70" s="30" t="s">
@@ -4389,7 +4377,7 @@
     </row>
     <row r="71" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A71" s="30"/>
-      <c r="C71" s="95"/>
+      <c r="C71" s="101"/>
       <c r="D71" s="30" t="s">
         <v>69</v>
       </c>
@@ -4399,7 +4387,7 @@
     </row>
     <row r="72" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A72" s="30"/>
-      <c r="C72" s="95"/>
+      <c r="C72" s="101"/>
       <c r="D72" s="30" t="s">
         <v>3</v>
       </c>
@@ -4409,7 +4397,7 @@
     </row>
     <row r="73" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A73" s="30"/>
-      <c r="C73" s="95"/>
+      <c r="C73" s="101"/>
       <c r="D73" s="30" t="s">
         <v>5</v>
       </c>
@@ -4419,7 +4407,7 @@
     </row>
     <row r="74" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A74" s="30"/>
-      <c r="C74" s="95"/>
+      <c r="C74" s="101"/>
       <c r="D74" s="30" t="s">
         <v>4</v>
       </c>
@@ -4430,7 +4418,7 @@
     <row r="75" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="31"/>
       <c r="B75" s="68"/>
-      <c r="C75" s="95"/>
+      <c r="C75" s="101"/>
       <c r="D75" s="31" t="s">
         <v>1</v>
       </c>
@@ -4441,17 +4429,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E46:E51"/>
-    <mergeCell ref="E39:E44"/>
-    <mergeCell ref="C64:C69"/>
-    <mergeCell ref="C70:C75"/>
-    <mergeCell ref="AN2:BR2"/>
     <mergeCell ref="BS2:CW2"/>
     <mergeCell ref="C33:C38"/>
     <mergeCell ref="C39:C44"/>
     <mergeCell ref="C46:C51"/>
     <mergeCell ref="C52:C57"/>
-    <mergeCell ref="C58:C63"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="C15:C20"/>
@@ -4459,6 +4441,12 @@
     <mergeCell ref="C27:C32"/>
     <mergeCell ref="J2:AM2"/>
     <mergeCell ref="F2:I2"/>
+    <mergeCell ref="E46:E51"/>
+    <mergeCell ref="E39:E44"/>
+    <mergeCell ref="C64:C69"/>
+    <mergeCell ref="C70:C75"/>
+    <mergeCell ref="AN2:BR2"/>
+    <mergeCell ref="C58:C63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>